<commit_message>
add bills analyze case
</commit_message>
<xml_diff>
--- a/output/xls/student.xlsx
+++ b/output/xls/student.xlsx
@@ -17,19 +17,19 @@
     <t>3</t>
   </si>
   <si>
-    <t>王五</t>
+    <t>鐜嬩簲</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>李四</t>
+    <t>鏉庡洓</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>张三</t>
+    <t>寮犱笁</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
add speech to text case
</commit_message>
<xml_diff>
--- a/output/xls/student.xlsx
+++ b/output/xls/student.xlsx
@@ -17,19 +17,19 @@
     <t>3</t>
   </si>
   <si>
-    <t>王五</t>
+    <t>鐜嬩簲</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>李四</t>
+    <t>鏉庡洓</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>张三</t>
+    <t>寮犱笁</t>
   </si>
 </sst>
 </file>

</xml_diff>